<commit_message>
Update ISPAuthorization Provider and creation output table
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
@@ -305,33 +305,6 @@
     <t>AVVIO_PROCEDUTA_CONCORSUALE_STRING</t>
   </si>
   <si>
-    <t xml:space="preserve">IND_1                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_2                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_3                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_4                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_5                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_6                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_7                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_8                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_9                         </t>
-  </si>
-  <si>
     <t xml:space="preserve">IND_10                        </t>
   </si>
   <si>
@@ -381,6 +354,33 @@
   </si>
   <si>
     <t>REAl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND_01                         </t>
+  </si>
+  <si>
+    <t>IND_02</t>
+  </si>
+  <si>
+    <t>IND_03</t>
+  </si>
+  <si>
+    <t>IND_04</t>
+  </si>
+  <si>
+    <t>IND_05</t>
+  </si>
+  <si>
+    <t>IND_06</t>
+  </si>
+  <si>
+    <t>IND_07</t>
+  </si>
+  <si>
+    <t>IND_08</t>
+  </si>
+  <si>
+    <t>IND_09</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1605,7 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1637,7 +1637,7 @@
         <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1669,7 +1669,7 @@
         <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1701,7 +1701,7 @@
         <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1733,7 +1733,7 @@
         <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1765,7 +1765,7 @@
         <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1797,7 +1797,7 @@
         <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -1829,7 +1829,7 @@
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -1861,7 +1861,7 @@
         <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -1876,7 +1876,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -1893,7 +1893,7 @@
         <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
@@ -1908,7 +1908,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -1925,7 +1925,7 @@
         <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -1940,7 +1940,7 @@
         <v>11</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -1957,22 +1957,22 @@
         <v>63</v>
       </c>
       <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="7">
+        <v>12</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="7">
-        <v>12</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -1989,7 +1989,7 @@
         <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -2004,7 +2004,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -2021,7 +2021,7 @@
         <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -2036,7 +2036,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -2044,16 +2044,16 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -2068,7 +2068,7 @@
         <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2132,10 +2132,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>42</v>
@@ -2285,10 +2285,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>59</v>
@@ -2387,16 +2387,16 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggionamento lib variable e analysis_Unit
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noemi.careddu\Desktop\Noemi\EW_BIB\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="656" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="656"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -395,36 +395,9 @@
     <t>JD_NEG_EV_PERS</t>
   </si>
   <si>
-    <t>IND_24</t>
-  </si>
-  <si>
     <t>JD_NEG_EV_PERS_STRING</t>
   </si>
   <si>
-    <t>IND_25</t>
-  </si>
-  <si>
-    <t>IND_26</t>
-  </si>
-  <si>
-    <t>IND_27</t>
-  </si>
-  <si>
-    <t>IND_28</t>
-  </si>
-  <si>
-    <t>IND_29</t>
-  </si>
-  <si>
-    <t>IND_30</t>
-  </si>
-  <si>
-    <t>IND_31</t>
-  </si>
-  <si>
-    <t>IND_32</t>
-  </si>
-  <si>
     <t>JD_PROTEST_INT</t>
   </si>
   <si>
@@ -452,30 +425,6 @@
     <t>24-Severe phenomena personnel management</t>
   </si>
   <si>
-    <t>25-Protested bill or our Bank initiative checks and other banks</t>
-  </si>
-  <si>
-    <t>26-Decanalization and issuance of convenience or abusive portfolio</t>
-  </si>
-  <si>
-    <t>27-Involvement in serious crimes with economic and legal consequences</t>
-  </si>
-  <si>
-    <t>28-Request admission to a competitive procedure for the debtor</t>
-  </si>
-  <si>
-    <t>29-Storage / Publication restructuring agreement for liquidation</t>
-  </si>
-  <si>
-    <t>30-Default with respect to payments on debt securities listed</t>
-  </si>
-  <si>
-    <t>31-Significant overdue debts towards public bodies</t>
-  </si>
-  <si>
-    <t>32-Initiation of bankruptcy proceedings for a group company</t>
-  </si>
-  <si>
     <t>JD_PROTEST_INT_STRING</t>
   </si>
   <si>
@@ -498,18 +447,76 @@
   </si>
   <si>
     <t>JD_CONCOR_AVVI_STRING</t>
+  </si>
+  <si>
+    <t>IND_15</t>
+  </si>
+  <si>
+    <t>IND_16</t>
+  </si>
+  <si>
+    <t>IND_17</t>
+  </si>
+  <si>
+    <t>IND_18</t>
+  </si>
+  <si>
+    <t>IND_19</t>
+  </si>
+  <si>
+    <t>IND_20</t>
+  </si>
+  <si>
+    <t>IND_21</t>
+  </si>
+  <si>
+    <t>IND_22</t>
+  </si>
+  <si>
+    <t>IND_23</t>
+  </si>
+  <si>
+    <t>16-Protested bill or our Bank initiative checks and other banks</t>
+  </si>
+  <si>
+    <t>17-Decanalization and issuance of convenience or abusive portfolio</t>
+  </si>
+  <si>
+    <t>18-Involvement in serious crimes with economic and legal consequences</t>
+  </si>
+  <si>
+    <t>19-Request admission to a competitive procedure for the debtor</t>
+  </si>
+  <si>
+    <t>20-Storage / Publication restructuring agreement for liquidation</t>
+  </si>
+  <si>
+    <t>21-Default with respect to payments on debt securities listed</t>
+  </si>
+  <si>
+    <t>22-Significant overdue debts towards public bodies</t>
+  </si>
+  <si>
+    <t>23-Initiation of bankruptcy proceedings for a group company</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -624,27 +631,28 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1672,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,11 +2390,11 @@
       <c r="D17" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>116</v>
+      <c r="E17" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G17" s="8">
         <v>24</v>
@@ -2418,19 +2426,19 @@
         <v>11</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>135</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G18" s="8">
         <v>25</v>
@@ -2462,19 +2470,19 @@
         <v>11</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>136</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="G19" s="8">
         <v>26</v>
@@ -2506,19 +2514,19 @@
         <v>11</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>137</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="G20" s="8">
         <v>27</v>
@@ -2550,19 +2558,19 @@
         <v>11</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>138</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="G21" s="8">
         <v>28</v>
@@ -2594,19 +2602,19 @@
         <v>11</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>139</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="G22" s="8">
         <v>29</v>
@@ -2638,19 +2646,19 @@
         <v>11</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>140</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>148</v>
       </c>
       <c r="G23" s="8">
         <v>30</v>
@@ -2682,19 +2690,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>141</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="G24" s="8">
         <v>31</v>
@@ -2726,19 +2734,19 @@
         <v>11</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="G25" s="8">
         <v>32</v>
@@ -2952,7 +2960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -3307,10 +3315,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>115</v>
@@ -3324,13 +3332,13 @@
         <v>11</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>23</v>
@@ -3341,13 +3349,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>23</v>
@@ -3358,13 +3366,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>23</v>
@@ -3375,13 +3383,13 @@
         <v>11</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>23</v>
@@ -3392,13 +3400,13 @@
         <v>11</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>23</v>
@@ -3409,13 +3417,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>23</v>
@@ -3426,13 +3434,13 @@
         <v>11</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>23</v>
@@ -3443,13 +3451,13 @@
         <v>11</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
aggiunti indicatori per semaforo di gruppo
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="r Variable_DataType" sheetId="3" r:id="rId2"/>
     <sheet name="Fields definition" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="733">
   <si>
     <t>Variable</t>
   </si>
@@ -2234,11 +2234,47 @@
   <si>
     <t>Il colore del modulo "Dati di Mercato" è dato dal SECONDO peggiore tra i semafori di categoria calcolati per EQUITY, CDS e BOND a seconda dei valori assunti dagli indicatori EDF_ImpliedRating, Bond_ImpliedRating e CDS_ImpliedRating</t>
   </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP1</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP2</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP3</t>
+  </si>
+  <si>
+    <t>QUOTA_EXP_GRP1</t>
+  </si>
+  <si>
+    <t>QUOTA_EXP_GRP2</t>
+  </si>
+  <si>
+    <t>QUOTA_EXP_GRP3</t>
+  </si>
+  <si>
+    <t>500 - QUOTA_EXP_GRP1</t>
+  </si>
+  <si>
+    <t>501 - QUOTA_EXP_GRP2</t>
+  </si>
+  <si>
+    <t>503 - QUOTA_EXP_GRP3</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP1_REAL</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP2_REAL</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP3_REAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2655,7 +2691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2778,6 +2814,13 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="47" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2875,7 +2918,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2561910</xdr:colOff>
+      <xdr:colOff>2109472</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>291387</xdr:rowOff>
     </xdr:to>
@@ -2933,7 +2976,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2561910</xdr:colOff>
+      <xdr:colOff>2109472</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>291387</xdr:rowOff>
     </xdr:to>
@@ -2991,7 +3034,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2561910</xdr:colOff>
+      <xdr:colOff>2109472</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>291387</xdr:rowOff>
     </xdr:to>
@@ -3049,7 +3092,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2561910</xdr:colOff>
+      <xdr:colOff>2109472</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>291387</xdr:rowOff>
     </xdr:to>
@@ -3107,7 +3150,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2561910</xdr:colOff>
+      <xdr:colOff>2109472</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>291387</xdr:rowOff>
     </xdr:to>
@@ -3616,6 +3659,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3651,6 +3711,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3803,26 +3880,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N163"/>
+  <dimension ref="A1:N166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="H137" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W144" sqref="W144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="58" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="1019" width="8.7109375"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="1019" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -10971,6 +11050,132 @@
         <v>0</v>
       </c>
     </row>
+    <row r="164" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A164" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="78" t="s">
+        <v>721</v>
+      </c>
+      <c r="C164" s="78" t="s">
+        <v>721</v>
+      </c>
+      <c r="D164" s="80"/>
+      <c r="E164" s="78" t="s">
+        <v>724</v>
+      </c>
+      <c r="F164" s="78" t="s">
+        <v>727</v>
+      </c>
+      <c r="G164" s="81">
+        <v>500</v>
+      </c>
+      <c r="H164" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I164" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J164" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="K164" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="L164" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="M164" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="N164" s="78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A165" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B165" s="78" t="s">
+        <v>722</v>
+      </c>
+      <c r="C165" s="78" t="s">
+        <v>722</v>
+      </c>
+      <c r="D165" s="80"/>
+      <c r="E165" s="78" t="s">
+        <v>725</v>
+      </c>
+      <c r="F165" s="78" t="s">
+        <v>728</v>
+      </c>
+      <c r="G165" s="81">
+        <v>501</v>
+      </c>
+      <c r="H165" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I165" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J165" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="K165" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="L165" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="M165" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="N165" s="78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A166" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B166" s="78" t="s">
+        <v>723</v>
+      </c>
+      <c r="C166" s="78" t="s">
+        <v>723</v>
+      </c>
+      <c r="D166" s="80"/>
+      <c r="E166" s="78" t="s">
+        <v>726</v>
+      </c>
+      <c r="F166" s="78" t="s">
+        <v>729</v>
+      </c>
+      <c r="G166" s="81">
+        <v>502</v>
+      </c>
+      <c r="H166" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I166" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J166" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="K166" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="L166" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="M166" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="N166" s="78" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -10980,10 +11185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H163"/>
+  <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A139" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13782,6 +13987,60 @@
         <v>478</v>
       </c>
       <c r="F163" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A164" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="78" t="s">
+        <v>730</v>
+      </c>
+      <c r="C164" s="78" t="s">
+        <v>730</v>
+      </c>
+      <c r="D164" s="78"/>
+      <c r="E164" s="78" t="s">
+        <v>721</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A165" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B165" s="78" t="s">
+        <v>731</v>
+      </c>
+      <c r="C165" s="78" t="s">
+        <v>731</v>
+      </c>
+      <c r="D165" s="78"/>
+      <c r="E165" s="78" t="s">
+        <v>722</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A166" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B166" s="78" t="s">
+        <v>732</v>
+      </c>
+      <c r="C166" s="78" t="s">
+        <v>732</v>
+      </c>
+      <c r="D166" s="78"/>
+      <c r="E166" s="78" t="s">
+        <v>723</v>
+      </c>
+      <c r="F166" s="4" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIX Exposure variable (oracle lock)
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="656" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="656"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -2699,7 +2699,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="63" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3525,7 +3525,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3583,7 +3589,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3641,7 +3653,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3699,7 +3717,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3757,7 +3781,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3815,7 +3845,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3863,7 +3899,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvPr id="13" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3921,7 +3963,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvPr id="14" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3979,7 +4027,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvPr id="15" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4037,7 +4091,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvPr id="16" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4095,7 +4155,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4153,7 +4219,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3074" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="3074" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4260,6 +4332,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4295,6 +4384,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4449,8 +4555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N221"/>
   <sheetViews>
-    <sheetView topLeftCell="E57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14171,8 +14277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove hidden columns: SNDG and exposure
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/02_Inst_Variable_fixed.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="874">
   <si>
     <t>Variable</t>
   </si>
@@ -4556,7 +4556,7 @@
   <dimension ref="A1:N221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4664,8 +4664,8 @@
       <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>13</v>
+      <c r="I3" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>101</v>
@@ -4709,7 +4709,7 @@
         <v>12</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>101</v>

</xml_diff>